<commit_message>
legujabb naplo, lehet boviteni
</commit_message>
<xml_diff>
--- a/naplo.xlsx
+++ b/naplo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Munka kezdete</t>
   </si>
@@ -33,10 +33,19 @@
     <t>Időtartam</t>
   </si>
   <si>
-    <t>Proba</t>
+    <t>Use-case diagramok szerkesztése</t>
   </si>
   <si>
-    <t>Csapat</t>
+    <t>Csomák Gábor, Jégh Tamás, Sziklay György, Vad Zsolt, Wiesner Péter</t>
+  </si>
+  <si>
+    <t>Követelmények, projektterv megfogalmazása</t>
+  </si>
+  <si>
+    <t>SZUMMA</t>
+  </si>
+  <si>
+    <t>Szótár készítése</t>
   </si>
 </sst>
 </file>
@@ -44,10 +53,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +73,12 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -73,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -181,51 +196,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -235,20 +279,137 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -264,6 +425,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -289,7 +451,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -317,8 +479,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -346,10 +507,12 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -373,6 +536,20 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="yyyy/\ m/\ d\.\ h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -382,6 +559,36 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -390,22 +597,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -427,15 +618,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Táblázat3" displayName="Táblázat3" ref="A1:E23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="5" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Táblázat3" displayName="Táblázat3" ref="A1:E24" totalsRowCount="1" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A1:E23"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Munka kezdete" dataDxfId="4"/>
-    <tableColumn id="2" name="Munka vége" dataDxfId="3"/>
-    <tableColumn id="3" name="Munka megnevezése" dataDxfId="2"/>
-    <tableColumn id="4" name="Résztvevők" dataDxfId="0"/>
-    <tableColumn id="5" name="Időtartam" dataDxfId="1">
+    <tableColumn id="1" name="Munka kezdete" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Munka vége" dataDxfId="8" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="Munka megnevezése" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="Résztvevők" dataDxfId="6" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="Időtartam" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="0">
       <calculatedColumnFormula>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM([Időtartam])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -727,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -758,42 +950,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="60">
       <c r="A2" s="3">
-        <v>40590.6875</v>
+        <v>40592.510416666664</v>
       </c>
       <c r="B2" s="4">
-        <v>40590.743055555555</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>40592.538194444445</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>5.5555555554747116E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
+      <c r="E2" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>2.7777777781011537E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60">
+      <c r="A3" s="3">
+        <v>40592.541666666664</v>
+      </c>
+      <c r="B3" s="4">
+        <v>40592.583333333336</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>4.1666666671517305E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60">
+      <c r="A4" s="3">
+        <v>40592.583333333336</v>
+      </c>
+      <c r="B4" s="4">
+        <v>40592.625</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>4.1666666664241347E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -801,7 +1009,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -811,7 +1019,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -821,7 +1029,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -831,7 +1039,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -841,7 +1049,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="2">
+      <c r="E9" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -851,7 +1059,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -861,7 +1069,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="2">
+      <c r="E11" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -871,7 +1079,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -881,7 +1089,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="2">
+      <c r="E13" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -891,7 +1099,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="2">
+      <c r="E14" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -901,7 +1109,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="2">
+      <c r="E15" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
         <v>0</v>
       </c>
@@ -911,79 +1119,91 @@
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="E16" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E17" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="E18" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="E19" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="E20" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="2">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
+      <c r="E23" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15">
+        <f>SUM([Időtartam])</f>
+        <v>0.11111111111677019</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
02 doksi (feladatleirason kivul) kesz naplo frissitve
</commit_message>
<xml_diff>
--- a/naplo.xlsx
+++ b/naplo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Munka kezdete</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Sziklay György</t>
+  </si>
+  <si>
+    <t>Szótár bővítése</t>
+  </si>
+  <si>
+    <t>Jégh Tamás, Vad Zsolt</t>
   </si>
 </sst>
 </file>
@@ -928,7 +934,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,7 +985,7 @@
         <v>40592.541666666664</v>
       </c>
       <c r="B3" s="4">
-        <v>40592.583333333336</v>
+        <v>40592.604166666664</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>7</v>
@@ -989,12 +995,12 @@
       </c>
       <c r="E3" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>4.1666666671517305E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60">
       <c r="A4" s="3">
-        <v>40592.583333333336</v>
+        <v>40592.604166666664</v>
       </c>
       <c r="B4" s="4">
         <v>40592.625</v>
@@ -1007,7 +1013,7 @@
       </c>
       <c r="E4" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>4.1666666664241347E-2</v>
+        <v>2.0833333335758653E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
@@ -1015,7 +1021,7 @@
         <v>40593.625</v>
       </c>
       <c r="B5" s="7">
-        <v>40593.638888888891</v>
+        <v>40593.652777777781</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>10</v>
@@ -1025,17 +1031,25 @@
       </c>
       <c r="E5" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>1.3888888890505768E-2</v>
+        <v>2.7777777781011537E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="A6" s="6">
+        <v>40594.972222222219</v>
+      </c>
+      <c r="B6" s="7">
+        <v>40595</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="E6" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
+        <v>2.7777777781011537E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1214,7 +1228,7 @@
       <c r="D24" s="14"/>
       <c r="E24" s="15">
         <f>SUM([Időtartam])</f>
-        <v>0.12500000000727596</v>
+        <v>0.16666666667879326</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
legfrisebb vegleges valtozat megtekintheto naplo frissitve
</commit_message>
<xml_diff>
--- a/naplo.xlsx
+++ b/naplo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Munka kezdete</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>Jégh Tamás, Vad Zsolt</t>
+  </si>
+  <si>
+    <t>Feladatleírás</t>
+  </si>
+  <si>
+    <t>Kockázatelemzés</t>
+  </si>
+  <si>
+    <t>Vad Zsolt</t>
+  </si>
+  <si>
+    <t>Jégh Tamás</t>
+  </si>
+  <si>
+    <t>Feladatleírás bővítése</t>
+  </si>
+  <si>
+    <t>Jégh Tamás, Wiesner Péter</t>
   </si>
 </sst>
 </file>
@@ -223,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -269,6 +287,15 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -934,7 +961,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,51 +1062,75 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6">
+      <c r="A6" s="16">
+        <v>40594.583333333336</v>
+      </c>
+      <c r="B6" s="17">
+        <v>40594.666666666664</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5">
+        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
+        <v>8.3333333328482695E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6">
         <v>40594.972222222219</v>
       </c>
-      <c r="B6" s="7">
-        <v>40595</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B7" s="7">
+        <v>40595.020833333336</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5">
-        <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>2.7777777781011537E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
       <c r="E7" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+        <v>4.8611111116770189E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="6">
+        <v>40595.027777777781</v>
+      </c>
+      <c r="B8" s="7">
+        <v>40595.055555555555</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
+        <v>2.7777777773735579E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="A9" s="6">
+        <v>40595.083333333336</v>
+      </c>
+      <c r="B9" s="7">
+        <v>40595.125</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="E9" s="5">
         <f>Táblázat3[[#This Row],[Munka vége]]-Táblázat3[[#This Row],[Munka kezdete]]</f>
-        <v>0</v>
+        <v>4.1666666664241347E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1228,7 +1279,7 @@
       <c r="D24" s="14"/>
       <c r="E24" s="15">
         <f>SUM([Időtartam])</f>
-        <v>0.16666666667879326</v>
+        <v>0.34027777778101154</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>

</xml_diff>